<commit_message>
Update liste de compo
</commit_message>
<xml_diff>
--- a/doc/Rapports/Liste de composants.xlsx
+++ b/doc/Rapports/Liste de composants.xlsx
@@ -91,27 +91,7 @@
     <t xml:space="preserve">https://fr.aliexpress.com/item/33006573082.html?_randl_currency=EUR&amp;_randl_shipto=FR&amp;src=google&amp;src=google&amp;albch=shopping&amp;acnt=248-630-5778&amp;slnk=&amp;plac=&amp;mtctp=&amp;albbt=Google_7_shopping&amp;gclsrc=aw.ds&amp;albagn=888888&amp;isSmbAutoCall=false&amp;needSmbHouyi=false&amp;src=google&amp;albch=shopping&amp;acnt=248-630-5778&amp;slnk=&amp;plac=&amp;mtctp=&amp;albbt=Google_7_shopping&amp;gclsrc=aw.ds&amp;albagn=888888&amp;ds_e_adid=609891816697&amp;ds_e_matchtype=&amp;ds_e_device=c&amp;ds_e_network=u&amp;ds_e_product_group_id=297309937645&amp;ds_e_product_id=fr33006573082&amp;ds_e_product_merchant_id=109338486&amp;ds_e_product_country=FR&amp;ds_e_product_language=fr&amp;ds_e_product_channel=online&amp;ds_e_product_store_id=&amp;ds_url_v=2&amp;albcp=17734099841&amp;albag=138402376763&amp;isSmbAutoCall=false&amp;needSmbHouyi=false&amp;gclid=Cj0KCQjwnbmaBhD-ARIsAGTPcfVA-9s_9EV0tEel0zyrJPGZgKcMZNkyZZ4BNZPjZz7d-VhZrpSIK4gaAouAEALw_wcB&amp;aff_fcid=a7ef4aa5f3894953875f3aece87cd67c-1666084659628-09809-UneMJZVf&amp;aff_fsk=UneMJZVf&amp;aff_platform=aaf&amp;sk=UneMJZVf&amp;aff_trace_key=a7ef4aa5f3894953875f3aece87cd67c-1666084659628-09809-UneMJZVf&amp;terminal_id=7109d70af6dc4a19a09bbe125bfd114d&amp;afSmartRedirect=y</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0563C1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Longueur MR106ZZ</t>
-    </r>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF0563C1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> /!\</t>
-    </r>
+    <t xml:space="preserve">Longueur MR106ZZ /!\</t>
   </si>
   <si>
     <t xml:space="preserve">Longueur: MR85ZZ /!\</t>
@@ -135,7 +115,7 @@
     <t xml:space="preserve">ZMR – ESC bidirectionnel sans balais 12A/20A/30A/40A/50A/60A/80A, pour voiture télécommandée, hélice sous marine pneumatique | AliExpress</t>
   </si>
   <si>
-    <t xml:space="preserve">Color: 4xESC with wires</t>
+    <t xml:space="preserve">Couleur: 40A (2-6S)</t>
   </si>
   <si>
     <t xml:space="preserve">Capteurs</t>
@@ -192,7 +172,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* \-??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,13 +209,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -532,7 +505,7 @@
   <dimension ref="A3:H36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>